<commit_message>
basic start to £RPI, $ARM and Semis
</commit_message>
<xml_diff>
--- a/£RPI.xlsx
+++ b/£RPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564B1336-28E6-474A-AF0D-0190664D256F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE68F7B-C3E8-43B0-AED5-BD2D6795C9DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="8475" xr2:uid="{455D1B8A-3F91-4588-9B7A-FCB01F8FFD95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="8475" activeTab="1" xr2:uid="{455D1B8A-3F91-4588-9B7A-FCB01F8FFD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0\x"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -835,42 +835,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -912,12 +876,6 @@
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -928,6 +886,48 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2395,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466F4785-7CF0-4D4B-866B-DCE268552EE9}">
   <dimension ref="B2:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2439,27 +2439,27 @@
       <c r="P3" s="25"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="G5" s="35" t="s">
+      <c r="C5" s="73"/>
+      <c r="D5" s="74"/>
+      <c r="G5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="37"/>
-      <c r="Q5" s="38" t="s">
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="74"/>
+      <c r="Q5" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
       <c r="X5" s="26" t="s">
         <v>29</v>
       </c>
@@ -2472,24 +2472,24 @@
         <v>3.2490000000000001</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="G6" s="77">
+      <c r="G6" s="63">
         <v>45536</v>
       </c>
-      <c r="H6" s="78" t="s">
+      <c r="H6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="79"/>
-      <c r="Q6" s="39" t="s">
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="65"/>
+      <c r="Q6" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -2503,13 +2503,13 @@
         <v>FY23</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="79"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
       <c r="Q7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2526,18 +2526,18 @@
         <v>628.40765803500005</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="G8" s="77">
+      <c r="G8" s="63">
         <v>45505</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="79"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="65"/>
       <c r="Q8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2558,13 +2558,13 @@
         <v>FY23</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="79"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
       <c r="Q9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2581,18 +2581,18 @@
         <f t="shared" si="0"/>
         <v>FY23</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="63">
         <v>45444</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="79"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="65"/>
       <c r="Q10" s="1" t="s">
         <v>136</v>
       </c>
@@ -2616,13 +2616,13 @@
         <v>FY23</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="79"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
       <c r="Q11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2640,13 +2640,13 @@
       </c>
       <c r="D12" s="15"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="79"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65"/>
       <c r="Q12" s="1" t="s">
         <v>128</v>
       </c>
@@ -2658,21 +2658,21 @@
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="74">
+      <c r="C13" s="60">
         <v>0.76</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="58"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="79"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
       <c r="Q13" s="1" t="s">
         <v>137</v>
       </c>
@@ -2682,67 +2682,67 @@
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G14" s="8"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="79"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65"/>
       <c r="Q14" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="74"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="79"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="65"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="67"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="79"/>
-      <c r="Q16" s="39" t="s">
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="65"/>
+      <c r="Q16" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
+      <c r="R16" s="76"/>
+      <c r="S16" s="76"/>
+      <c r="T16" s="76"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="79"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="65"/>
       <c r="Q17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2754,20 +2754,20 @@
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="79"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="65"/>
       <c r="Q18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W18" s="56" t="s">
+      <c r="W18" s="44" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2775,57 +2775,57 @@
       <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="78"/>
       <c r="G19" s="8">
         <v>2012</v>
       </c>
-      <c r="H19" s="78" t="s">
+      <c r="H19" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="79"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="65"/>
       <c r="Q19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X19" s="56"/>
+      <c r="X19" s="44"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G20" s="8"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="79"/>
-      <c r="X20" s="56"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="65"/>
+      <c r="X20" s="44"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G21" s="8">
         <v>2009</v>
       </c>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="78"/>
-      <c r="N21" s="79"/>
-      <c r="X21" s="56"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="65"/>
+      <c r="X21" s="44"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="74"/>
       <c r="G22" s="9"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
@@ -2839,20 +2839,20 @@
       <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="67"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="66">
         <v>2012</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="62" t="s">
+      <c r="D24" s="67"/>
+      <c r="E24" s="50" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2860,25 +2860,25 @@
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="79">
         <v>45444</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="67"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="67"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="66">
         <f>+'Financial Model'!K50</f>
         <v>103</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="67"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
@@ -2897,73 +2897,73 @@
       <c r="C30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="76"/>
+      <c r="D30" s="62"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B31" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="34"/>
+      <c r="D31" s="71"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="74"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="70">
+      <c r="C35" s="68">
         <f>C6/'Financial Model'!K88</f>
         <v>1.2244021194329087E-2</v>
       </c>
-      <c r="D35" s="71"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="70">
+      <c r="C36" s="68">
         <f>+C8/('Financial Model'!K13*Main!C13)</f>
         <v>3.110840911014797</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="69"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="70">
+      <c r="C37" s="68">
         <f>+C12/('Financial Model'!K13*Main!C13)</f>
         <v>2.9337073130156908</v>
       </c>
-      <c r="D37" s="71"/>
+      <c r="D37" s="69"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="70">
+      <c r="C38" s="68">
         <f>+C6/('Financial Model'!K26*Main!C13)</f>
         <v>15.061074686431013</v>
       </c>
-      <c r="D38" s="71"/>
+      <c r="D38" s="69"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="70">
+      <c r="C39" s="68">
         <f>C12/('Financial Model'!K25*Main!C13)</f>
         <v>24.698169348715048</v>
       </c>
-      <c r="D39" s="71"/>
+      <c r="D39" s="69"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="8"/>
@@ -2982,6 +2982,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Q16:T16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
@@ -2993,18 +3001,10 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{C8D4D434-582F-463A-A9FE-87E24B6B9D24}"/>
@@ -3019,11 +3019,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A18B329-9CBE-49D8-B2AA-D4DBC0BF2B3C}">
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3036,7 +3036,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -3067,10 +3067,10 @@
     <row r="2" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
       <c r="E2" s="29"/>
-      <c r="I2" s="44">
+      <c r="I2" s="32">
         <v>44561</v>
       </c>
-      <c r="J2" s="44">
+      <c r="J2" s="32">
         <v>44926</v>
       </c>
       <c r="K2" s="18" t="s">
@@ -3081,63 +3081,63 @@
       <c r="A3" s="19"/>
       <c r="E3" s="29"/>
     </row>
-    <row r="4" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="64" t="s">
+    <row r="4" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="I4" s="66">
+      <c r="E4" s="53"/>
+      <c r="I4" s="54">
         <v>75.173000000000002</v>
       </c>
-      <c r="J4" s="66">
+      <c r="J4" s="54">
         <v>64.546000000000006</v>
       </c>
-      <c r="K4" s="66">
+      <c r="K4" s="54">
         <v>104.75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+    <row r="5" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="I5" s="66">
+      <c r="E5" s="53"/>
+      <c r="I5" s="54">
         <v>12.337</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="54">
         <v>30.446999999999999</v>
       </c>
-      <c r="K5" s="66">
+      <c r="K5" s="54">
         <v>45.277999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="64" t="s">
+    <row r="6" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="I6" s="66">
+      <c r="E6" s="53"/>
+      <c r="I6" s="54">
         <v>22.186</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="54">
         <v>49.491999999999997</v>
       </c>
-      <c r="K6" s="66">
+      <c r="K6" s="54">
         <v>60.317</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="64" t="s">
+    <row r="7" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="I7" s="66">
+      <c r="E7" s="53"/>
+      <c r="I7" s="54">
         <v>30.890999999999998</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="54">
         <v>43.374000000000002</v>
       </c>
-      <c r="K7" s="66">
+      <c r="K7" s="54">
         <v>55.451999999999998</v>
       </c>
     </row>
@@ -3145,74 +3145,74 @@
       <c r="B8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="I8" s="67" t="s">
+      <c r="E8" s="31"/>
+      <c r="I8" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="67" t="s">
+      <c r="K8" s="55" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="64" t="s">
+    <row r="9" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="65"/>
-      <c r="I9" s="66">
+      <c r="E9" s="53"/>
+      <c r="I9" s="54">
         <v>83.522999999999996</v>
       </c>
-      <c r="J9" s="66">
+      <c r="J9" s="54">
         <v>150.065</v>
       </c>
-      <c r="K9" s="66">
+      <c r="K9" s="54">
         <v>212.279</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="64" t="s">
+    <row r="10" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="I10" s="66">
+      <c r="E10" s="53"/>
+      <c r="I10" s="54">
         <v>26.780999999999999</v>
       </c>
-      <c r="J10" s="66">
+      <c r="J10" s="54">
         <v>9.5730000000000004</v>
       </c>
-      <c r="K10" s="66">
+      <c r="K10" s="54">
         <v>8.7870000000000008</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="64" t="s">
+    <row r="11" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="I11" s="66">
+      <c r="E11" s="53"/>
+      <c r="I11" s="54">
         <v>28.062999999999999</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="54">
         <v>26.591000000000001</v>
       </c>
-      <c r="K11" s="66">
+      <c r="K11" s="54">
         <v>43.484000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="64" t="s">
+    <row r="12" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="I12" s="66">
+      <c r="E12" s="53"/>
+      <c r="I12" s="54">
         <v>2.2200000000000002</v>
       </c>
-      <c r="J12" s="66">
+      <c r="J12" s="54">
         <v>1.63</v>
       </c>
-      <c r="K12" s="66">
+      <c r="K12" s="54">
         <v>1.2470000000000001</v>
       </c>
     </row>
@@ -3220,14 +3220,14 @@
       <c r="B13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="I13" s="46">
+      <c r="E13" s="31"/>
+      <c r="I13" s="34">
         <v>140.58699999999999</v>
       </c>
-      <c r="J13" s="46">
+      <c r="J13" s="34">
         <v>187.85900000000001</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="34">
         <v>265.79700000000003</v>
       </c>
     </row>
@@ -3235,13 +3235,13 @@
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="35">
         <v>98.67</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="35">
         <v>145.57900000000001</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="35">
         <v>199.84200000000001</v>
       </c>
     </row>
@@ -3249,16 +3249,16 @@
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="I15" s="46">
+      <c r="E15" s="31"/>
+      <c r="I15" s="34">
         <f>+I13-I14</f>
         <v>41.916999999999987</v>
       </c>
-      <c r="J15" s="46">
+      <c r="J15" s="34">
         <f>+J13-J14</f>
         <v>42.28</v>
       </c>
-      <c r="K15" s="46">
+      <c r="K15" s="34">
         <f>+K13-K14</f>
         <v>65.955000000000013</v>
       </c>
@@ -3267,13 +3267,13 @@
       <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="35">
         <v>11.792999999999999</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="35">
         <v>13.794</v>
       </c>
-      <c r="K16" s="47">
+      <c r="K16" s="35">
         <v>17.649999999999999</v>
       </c>
     </row>
@@ -3281,13 +3281,13 @@
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="35">
         <v>11.124000000000001</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="35">
         <v>9.2509999999999994</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="35">
         <v>10.582000000000001</v>
       </c>
     </row>
@@ -3295,13 +3295,13 @@
       <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="35">
         <v>-0.27200000000000002</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="35">
         <v>0.83299999999999996</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="35">
         <v>-0.191</v>
       </c>
     </row>
@@ -3309,13 +3309,13 @@
       <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="35">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="35">
         <v>0</v>
       </c>
-      <c r="K19" s="47">
+      <c r="K19" s="35">
         <v>0</v>
       </c>
     </row>
@@ -3323,16 +3323,16 @@
       <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="I20" s="46">
+      <c r="E20" s="31"/>
+      <c r="I20" s="34">
         <f t="shared" ref="I20:J20" si="0">+I15-I16-I17+I18+I19</f>
         <v>18.764999999999986</v>
       </c>
-      <c r="J20" s="46">
+      <c r="J20" s="34">
         <f t="shared" si="0"/>
         <v>20.067999999999998</v>
       </c>
-      <c r="K20" s="46">
+      <c r="K20" s="34">
         <f>+K15-K16-K17+K18+K19</f>
         <v>37.532000000000011</v>
       </c>
@@ -3341,13 +3341,13 @@
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="47">
+      <c r="I21" s="35">
         <v>0</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="35">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="K21" s="47">
+      <c r="K21" s="35">
         <v>1.4430000000000001</v>
       </c>
     </row>
@@ -3355,13 +3355,13 @@
       <c r="B22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="35">
         <v>0.29199999999999998</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="35">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="K22" s="47">
+      <c r="K22" s="35">
         <v>0.77900000000000003</v>
       </c>
     </row>
@@ -3369,15 +3369,15 @@
       <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="47">
+      <c r="I23" s="35">
         <f t="shared" ref="I23:J23" si="1">+I20+I21-I22</f>
         <v>18.472999999999985</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="35">
         <f t="shared" si="1"/>
         <v>20.087999999999997</v>
       </c>
-      <c r="K23" s="47">
+      <c r="K23" s="35">
         <f>+K20+K21-K22</f>
         <v>38.196000000000005</v>
       </c>
@@ -3386,13 +3386,13 @@
       <c r="B24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="47">
+      <c r="I24" s="35">
         <v>3.6219999999999999</v>
       </c>
-      <c r="J24" s="47">
+      <c r="J24" s="35">
         <v>3.0209999999999999</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K24" s="35">
         <v>6.6239999999999997</v>
       </c>
     </row>
@@ -3400,208 +3400,208 @@
       <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="I25" s="46">
+      <c r="E25" s="31"/>
+      <c r="I25" s="34">
         <f t="shared" ref="I25:J25" si="2">+I23-I24</f>
         <v>14.850999999999985</v>
       </c>
-      <c r="J25" s="46">
+      <c r="J25" s="34">
         <f t="shared" si="2"/>
         <v>17.066999999999997</v>
       </c>
-      <c r="K25" s="46">
+      <c r="K25" s="34">
         <f>+K23-K24</f>
         <v>31.572000000000006</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="52" t="s">
+    <row r="26" spans="2:11" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="I26" s="52">
+      <c r="E26" s="41"/>
+      <c r="I26" s="40">
         <f>I25/I27</f>
         <v>0.14404182266105395</v>
       </c>
-      <c r="J26" s="52">
+      <c r="J26" s="40">
         <f>J25/J27</f>
         <v>0.15525193075656546</v>
       </c>
-      <c r="K26" s="52">
+      <c r="K26" s="40">
         <f>K25/K27</f>
         <v>0.28384428661332378</v>
       </c>
     </row>
-    <row r="27" spans="2:11" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="47" t="s">
+    <row r="27" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="54"/>
-      <c r="I27" s="47">
+      <c r="E27" s="42"/>
+      <c r="I27" s="35">
         <v>103.102</v>
       </c>
-      <c r="J27" s="47">
+      <c r="J27" s="35">
         <v>109.931</v>
       </c>
-      <c r="K27" s="47">
+      <c r="K27" s="35">
         <v>111.23</v>
       </c>
     </row>
-    <row r="30" spans="2:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="48" t="s">
+    <row r="30" spans="2:11" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="49"/>
-      <c r="I30" s="50" t="s">
+      <c r="E30" s="37"/>
+      <c r="I30" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J30" s="48">
+      <c r="J30" s="36">
         <f>J13/I13-1</f>
         <v>0.33624730593867169</v>
       </c>
-      <c r="K30" s="48">
+      <c r="K30" s="36">
         <f>K13/J13-1</f>
         <v>0.41487498602675421</v>
       </c>
     </row>
-    <row r="31" spans="2:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="64" t="s">
+    <row r="31" spans="2:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="69"/>
-      <c r="I31" s="50" t="s">
+      <c r="E31" s="57"/>
+      <c r="I31" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J31" s="68">
-        <f>J4/I4-1</f>
+      <c r="J31" s="56">
+        <f t="shared" ref="J31:K34" si="3">J4/I4-1</f>
         <v>-0.1413672462187221</v>
       </c>
-      <c r="K31" s="68">
-        <f>K4/J4-1</f>
+      <c r="K31" s="56">
+        <f t="shared" si="3"/>
         <v>0.62287360951879256</v>
       </c>
     </row>
-    <row r="32" spans="2:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="64" t="s">
+    <row r="32" spans="2:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="69"/>
-      <c r="I32" s="50" t="s">
+      <c r="E32" s="57"/>
+      <c r="I32" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J32" s="68">
-        <f>J5/I5-1</f>
+      <c r="J32" s="56">
+        <f t="shared" si="3"/>
         <v>1.4679419632001296</v>
       </c>
-      <c r="K32" s="68">
-        <f>K5/J5-1</f>
+      <c r="K32" s="56">
+        <f t="shared" si="3"/>
         <v>0.48710874634610968</v>
       </c>
     </row>
-    <row r="33" spans="2:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="64" t="s">
+    <row r="33" spans="2:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="69"/>
-      <c r="I33" s="50" t="s">
+      <c r="E33" s="57"/>
+      <c r="I33" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J33" s="68">
-        <f>J6/I6-1</f>
+      <c r="J33" s="56">
+        <f t="shared" si="3"/>
         <v>1.2307761651491931</v>
       </c>
-      <c r="K33" s="68">
-        <f>K6/J6-1</f>
+      <c r="K33" s="56">
+        <f t="shared" si="3"/>
         <v>0.21872221773215883</v>
       </c>
     </row>
-    <row r="34" spans="2:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="64" t="s">
+    <row r="34" spans="2:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="69"/>
-      <c r="I34" s="50" t="s">
+      <c r="E34" s="57"/>
+      <c r="I34" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="68">
-        <f>J7/I7-1</f>
+      <c r="J34" s="56">
+        <f t="shared" si="3"/>
         <v>0.40409828105273404</v>
       </c>
-      <c r="K34" s="68">
-        <f>K7/J7-1</f>
+      <c r="K34" s="56">
+        <f t="shared" si="3"/>
         <v>0.2784617512795684</v>
       </c>
     </row>
-    <row r="35" spans="2:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="75" t="s">
+    <row r="35" spans="2:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="69"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
+      <c r="E35" s="57"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="I36" s="50" t="s">
+      <c r="I36" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J36" s="68">
-        <f>J9/I9-1</f>
+      <c r="J36" s="56">
+        <f t="shared" ref="J36:K39" si="4">J9/I9-1</f>
         <v>0.79669073189420891</v>
       </c>
-      <c r="K36" s="68">
-        <f>K9/J9-1</f>
+      <c r="K36" s="56">
+        <f t="shared" si="4"/>
         <v>0.41458034851564318</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="I37" s="50" t="s">
+      <c r="I37" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J37" s="68">
-        <f>J10/I10-1</f>
+      <c r="J37" s="56">
+        <f t="shared" si="4"/>
         <v>-0.6425450879354766</v>
       </c>
-      <c r="K37" s="68">
-        <f>K10/J10-1</f>
+      <c r="K37" s="56">
+        <f t="shared" si="4"/>
         <v>-8.2105922908179196E-2</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I38" s="50" t="s">
+      <c r="I38" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J38" s="68">
-        <f>J11/I11-1</f>
+      <c r="J38" s="56">
+        <f t="shared" si="4"/>
         <v>-5.2453408402522772E-2</v>
       </c>
-      <c r="K38" s="68">
-        <f>K11/J11-1</f>
+      <c r="K38" s="56">
+        <f t="shared" si="4"/>
         <v>0.63529013576021964</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="I39" s="50" t="s">
+      <c r="I39" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J39" s="68">
-        <f>J12/I12-1</f>
+      <c r="J39" s="56">
+        <f t="shared" si="4"/>
         <v>-0.26576576576576583</v>
       </c>
-      <c r="K39" s="68">
-        <f>K12/J12-1</f>
+      <c r="K39" s="56">
+        <f t="shared" si="4"/>
         <v>-0.2349693251533741</v>
       </c>
     </row>
@@ -3609,13 +3609,13 @@
       <c r="B40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I40" s="50" t="s">
+      <c r="I40" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J40" s="50" t="s">
+      <c r="J40" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="K40" s="50" t="s">
+      <c r="K40" s="38" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3623,15 +3623,15 @@
       <c r="B42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I42" s="51">
+      <c r="I42" s="39">
         <f>I15/I13</f>
         <v>0.29815701309509407</v>
       </c>
-      <c r="J42" s="51">
+      <c r="J42" s="39">
         <f>J15/J13</f>
         <v>0.22506241383165032</v>
       </c>
-      <c r="K42" s="51">
+      <c r="K42" s="39">
         <f>K15/K13</f>
         <v>0.24814049819975398</v>
       </c>
@@ -3640,15 +3640,15 @@
       <c r="B43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I43" s="51">
+      <c r="I43" s="39">
         <f>I20/I13</f>
         <v>0.13347606819976235</v>
       </c>
-      <c r="J43" s="51">
+      <c r="J43" s="39">
         <f>J20/J13</f>
         <v>0.10682479945065181</v>
       </c>
-      <c r="K43" s="51">
+      <c r="K43" s="39">
         <f>K20/K13</f>
         <v>0.14120550645793598</v>
       </c>
@@ -3657,15 +3657,15 @@
       <c r="B44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I44" s="51">
+      <c r="I44" s="39">
         <f>I25/I13</f>
         <v>0.10563565621287876</v>
       </c>
-      <c r="J44" s="51">
+      <c r="J44" s="39">
         <f>J25/J13</f>
         <v>9.0850052432941711E-2</v>
       </c>
-      <c r="K44" s="51">
+      <c r="K44" s="39">
         <f>K25/K13</f>
         <v>0.11878237903362342</v>
       </c>
@@ -3674,21 +3674,21 @@
       <c r="B45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="51">
-        <f t="shared" ref="I45:K45" si="3">I24/I23</f>
+      <c r="I45" s="39">
+        <f t="shared" ref="I45:J45" si="5">I24/I23</f>
         <v>0.19606993991230459</v>
       </c>
-      <c r="J45" s="51">
-        <f t="shared" si="3"/>
+      <c r="J45" s="39">
+        <f t="shared" si="5"/>
         <v>0.1503882915173238</v>
       </c>
-      <c r="K45" s="51">
+      <c r="K45" s="39">
         <f>K24/K23</f>
         <v>0.17342130065975492</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="55" t="s">
+      <c r="B49" s="43" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3696,7 +3696,7 @@
       <c r="B50" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="43"/>
+      <c r="E50" s="31"/>
       <c r="I50" s="2">
         <f>SUM(I51:I56)</f>
         <v>85</v>
@@ -3710,115 +3710,115 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="57" t="s">
+    <row r="51" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="59"/>
-      <c r="I51" s="58">
+      <c r="E51" s="47"/>
+      <c r="I51" s="46">
         <v>39</v>
       </c>
-      <c r="J51" s="58">
+      <c r="J51" s="46">
         <v>44</v>
       </c>
-      <c r="K51" s="58">
+      <c r="K51" s="46">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="57" t="s">
+    <row r="52" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="59"/>
-      <c r="I52" s="58">
+      <c r="E52" s="47"/>
+      <c r="I52" s="46">
         <v>14</v>
       </c>
-      <c r="J52" s="58">
+      <c r="J52" s="46">
         <v>16</v>
       </c>
-      <c r="K52" s="58">
+      <c r="K52" s="46">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="57" t="s">
+    <row r="53" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="59"/>
-      <c r="I53" s="58">
+      <c r="E53" s="47"/>
+      <c r="I53" s="46">
         <v>8</v>
       </c>
-      <c r="J53" s="58">
+      <c r="J53" s="46">
         <v>10</v>
       </c>
-      <c r="K53" s="58">
+      <c r="K53" s="46">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="57" t="s">
+    <row r="54" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E54" s="59"/>
-      <c r="I54" s="58">
+      <c r="E54" s="47"/>
+      <c r="I54" s="46">
         <v>10</v>
       </c>
-      <c r="J54" s="58">
+      <c r="J54" s="46">
         <v>10</v>
       </c>
-      <c r="K54" s="58">
+      <c r="K54" s="46">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="57" t="s">
+    <row r="55" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="E55" s="59"/>
-      <c r="I55" s="58">
+      <c r="E55" s="47"/>
+      <c r="I55" s="46">
         <v>10</v>
       </c>
-      <c r="J55" s="58">
+      <c r="J55" s="46">
         <v>12</v>
       </c>
-      <c r="K55" s="58">
+      <c r="K55" s="46">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="57" t="s">
+    <row r="56" spans="2:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E56" s="59"/>
-      <c r="I56" s="58">
+      <c r="E56" s="47"/>
+      <c r="I56" s="46">
         <v>4</v>
       </c>
-      <c r="J56" s="58">
+      <c r="J56" s="46">
         <v>4</v>
       </c>
-      <c r="K56" s="58">
+      <c r="K56" s="46">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="60" t="s">
+    <row r="57" spans="2:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="E57" s="61"/>
-      <c r="I57" s="50" t="s">
+      <c r="E57" s="49"/>
+      <c r="I57" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J57" s="60">
+      <c r="J57" s="48">
         <f>J50/I50-1</f>
         <v>0.12941176470588234</v>
       </c>
-      <c r="K57" s="60">
+      <c r="K57" s="48">
         <f>K50/J50-1</f>
         <v>7.2916666666666741E-2</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="55" t="s">
+      <c r="B61" s="43" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3826,13 +3826,13 @@
       <c r="B62" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I62" s="47">
+      <c r="I62" s="35">
         <v>25.806999999999999</v>
       </c>
-      <c r="J62" s="47">
+      <c r="J62" s="35">
         <v>35.534999999999997</v>
       </c>
-      <c r="K62" s="47">
+      <c r="K62" s="35">
         <v>58.634</v>
       </c>
     </row>
@@ -3840,13 +3840,13 @@
       <c r="B63" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I63" s="47">
+      <c r="I63" s="35">
         <v>3.5590000000000002</v>
       </c>
-      <c r="J63" s="47">
+      <c r="J63" s="35">
         <v>3.7210000000000001</v>
       </c>
-      <c r="K63" s="47">
+      <c r="K63" s="35">
         <v>5.0780000000000003</v>
       </c>
     </row>
@@ -3854,13 +3854,13 @@
       <c r="B64" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I64" s="47">
+      <c r="I64" s="35">
         <v>1.679</v>
       </c>
-      <c r="J64" s="47">
+      <c r="J64" s="35">
         <v>1.387</v>
       </c>
-      <c r="K64" s="47">
+      <c r="K64" s="35">
         <v>6.7190000000000003</v>
       </c>
     </row>
@@ -3868,13 +3868,13 @@
       <c r="B65" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I65" s="47">
+      <c r="I65" s="35">
         <v>0</v>
       </c>
-      <c r="J65" s="47">
+      <c r="J65" s="35">
         <v>0</v>
       </c>
-      <c r="K65" s="47">
+      <c r="K65" s="35">
         <v>2.698</v>
       </c>
     </row>
@@ -3882,15 +3882,15 @@
       <c r="B66" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I66" s="47">
-        <f t="shared" ref="I66:J66" si="4">+SUM(I62:I65)</f>
+      <c r="I66" s="35">
+        <f t="shared" ref="I66:J66" si="6">+SUM(I62:I65)</f>
         <v>31.044999999999998</v>
       </c>
-      <c r="J66" s="47">
-        <f t="shared" si="4"/>
+      <c r="J66" s="35">
+        <f t="shared" si="6"/>
         <v>40.643000000000001</v>
       </c>
-      <c r="K66" s="47">
+      <c r="K66" s="35">
         <f>+SUM(K62:K65)</f>
         <v>73.128999999999991</v>
       </c>
@@ -3899,14 +3899,14 @@
       <c r="B67" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E67" s="43"/>
-      <c r="I67" s="46">
+      <c r="E67" s="31"/>
+      <c r="I67" s="34">
         <v>40.576000000000001</v>
       </c>
-      <c r="J67" s="46">
+      <c r="J67" s="34">
         <v>47.889000000000003</v>
       </c>
-      <c r="K67" s="46">
+      <c r="K67" s="34">
         <v>108.057</v>
       </c>
     </row>
@@ -3914,13 +3914,13 @@
       <c r="B68" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I68" s="47">
+      <c r="I68" s="35">
         <v>20.734000000000002</v>
       </c>
-      <c r="J68" s="47">
+      <c r="J68" s="35">
         <v>26.027000000000001</v>
       </c>
-      <c r="K68" s="47">
+      <c r="K68" s="35">
         <v>39.76</v>
       </c>
     </row>
@@ -3928,14 +3928,14 @@
       <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="43"/>
-      <c r="I69" s="46">
+      <c r="E69" s="31"/>
+      <c r="I69" s="34">
         <v>34.429000000000002</v>
       </c>
-      <c r="J69" s="46">
+      <c r="J69" s="34">
         <v>32.843000000000004</v>
       </c>
-      <c r="K69" s="46">
+      <c r="K69" s="34">
         <v>42.207000000000001</v>
       </c>
     </row>
@@ -3943,13 +3943,13 @@
       <c r="B70" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I70" s="47">
+      <c r="I70" s="35">
         <v>0</v>
       </c>
-      <c r="J70" s="47">
+      <c r="J70" s="35">
         <v>0</v>
       </c>
-      <c r="K70" s="47">
+      <c r="K70" s="35">
         <v>2.2010000000000001</v>
       </c>
     </row>
@@ -3957,35 +3957,35 @@
       <c r="B71" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I71" s="47">
-        <f t="shared" ref="I71:J71" si="5">+I66+SUM(I67:I70)</f>
+      <c r="I71" s="35">
+        <f t="shared" ref="I71:J71" si="7">+I66+SUM(I67:I70)</f>
         <v>126.78400000000001</v>
       </c>
-      <c r="J71" s="47">
-        <f t="shared" si="5"/>
+      <c r="J71" s="35">
+        <f t="shared" si="7"/>
         <v>147.40199999999999</v>
       </c>
-      <c r="K71" s="47">
+      <c r="K71" s="35">
         <f>+K66+SUM(K67:K70)</f>
         <v>265.35399999999998</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="I72" s="47"/>
-      <c r="J72" s="47"/>
-      <c r="K72" s="47"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I73" s="47">
+      <c r="I73" s="35">
         <v>22.542999999999999</v>
       </c>
-      <c r="J73" s="47">
+      <c r="J73" s="35">
         <v>26.494</v>
       </c>
-      <c r="K73" s="47">
+      <c r="K73" s="35">
         <v>81.19</v>
       </c>
     </row>
@@ -3993,13 +3993,13 @@
       <c r="B74" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I74" s="47">
+      <c r="I74" s="35">
         <v>0</v>
       </c>
-      <c r="J74" s="47">
+      <c r="J74" s="35">
         <v>0</v>
       </c>
-      <c r="K74" s="47">
+      <c r="K74" s="35">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -4007,13 +4007,13 @@
       <c r="B75" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I75" s="47">
+      <c r="I75" s="35">
         <v>0.16500000000000001</v>
       </c>
-      <c r="J75" s="47">
+      <c r="J75" s="35">
         <v>0.26300000000000001</v>
       </c>
-      <c r="K75" s="47">
+      <c r="K75" s="35">
         <v>1.252</v>
       </c>
     </row>
@@ -4021,13 +4021,13 @@
       <c r="B76" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I76" s="47">
+      <c r="I76" s="35">
         <v>0.39</v>
       </c>
-      <c r="J76" s="47">
+      <c r="J76" s="35">
         <v>0.76200000000000001</v>
       </c>
-      <c r="K76" s="47">
+      <c r="K76" s="35">
         <v>0</v>
       </c>
     </row>
@@ -4035,15 +4035,15 @@
       <c r="B77" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I77" s="47">
-        <f t="shared" ref="I77:J77" si="6">SUM(I73:I76)</f>
+      <c r="I77" s="35">
+        <f t="shared" ref="I77:J77" si="8">SUM(I73:I76)</f>
         <v>23.097999999999999</v>
       </c>
-      <c r="J77" s="47">
-        <f t="shared" si="6"/>
+      <c r="J77" s="35">
+        <f t="shared" si="8"/>
         <v>27.519000000000002</v>
       </c>
-      <c r="K77" s="47">
+      <c r="K77" s="35">
         <f>SUM(K73:K76)</f>
         <v>82.886999999999986</v>
       </c>
@@ -4052,13 +4052,13 @@
       <c r="B78" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I78" s="47">
+      <c r="I78" s="35">
         <v>1.9510000000000001</v>
       </c>
-      <c r="J78" s="47">
+      <c r="J78" s="35">
         <v>1.359</v>
       </c>
-      <c r="K78" s="47">
+      <c r="K78" s="35">
         <v>5.8280000000000003</v>
       </c>
     </row>
@@ -4066,13 +4066,13 @@
       <c r="B79" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I79" s="47">
+      <c r="I79" s="35">
         <v>6.2140000000000004</v>
       </c>
-      <c r="J79" s="47">
+      <c r="J79" s="35">
         <v>7.673</v>
       </c>
-      <c r="K79" s="47">
+      <c r="K79" s="35">
         <v>10.244</v>
       </c>
     </row>
@@ -4080,13 +4080,13 @@
       <c r="B80" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I80" s="47">
+      <c r="I80" s="35">
         <v>0</v>
       </c>
-      <c r="J80" s="47">
+      <c r="J80" s="35">
         <v>3.7</v>
       </c>
-      <c r="K80" s="47">
+      <c r="K80" s="35">
         <v>6.4249999999999998</v>
       </c>
     </row>
@@ -4094,13 +4094,13 @@
       <c r="B81" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I81" s="47">
+      <c r="I81" s="35">
         <v>0</v>
       </c>
-      <c r="J81" s="47">
+      <c r="J81" s="35">
         <v>0</v>
       </c>
-      <c r="K81" s="47">
+      <c r="K81" s="35">
         <v>0.75600000000000001</v>
       </c>
     </row>
@@ -4108,36 +4108,36 @@
       <c r="B82" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E82" s="43"/>
-      <c r="I82" s="46">
-        <f t="shared" ref="I82:J82" si="7">SUM(I77:I81)</f>
+      <c r="E82" s="31"/>
+      <c r="I82" s="34">
+        <f t="shared" ref="I82:J82" si="9">SUM(I77:I81)</f>
         <v>31.262999999999998</v>
       </c>
-      <c r="J82" s="46">
-        <f t="shared" si="7"/>
+      <c r="J82" s="34">
+        <f t="shared" si="9"/>
         <v>40.251000000000005</v>
       </c>
-      <c r="K82" s="46">
+      <c r="K82" s="34">
         <f>SUM(K77:K81)</f>
         <v>106.13999999999999</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="I83" s="47"/>
-      <c r="J83" s="47"/>
-      <c r="K83" s="47"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="35"/>
+      <c r="K83" s="35"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I84" s="47">
+      <c r="I84" s="35">
         <v>95.521000000000001</v>
       </c>
-      <c r="J84" s="47">
+      <c r="J84" s="35">
         <v>107.151</v>
       </c>
-      <c r="K84" s="47">
+      <c r="K84" s="35">
         <v>159.214</v>
       </c>
     </row>
@@ -4145,36 +4145,36 @@
       <c r="B85" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I85" s="47">
+      <c r="I85" s="35">
         <f>+I84+I82</f>
         <v>126.78399999999999</v>
       </c>
-      <c r="J85" s="47">
+      <c r="J85" s="35">
         <f>+J84+J82</f>
         <v>147.40199999999999</v>
       </c>
-      <c r="K85" s="47">
+      <c r="K85" s="35">
         <f>+K84+K82</f>
         <v>265.35399999999998</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="I86" s="47"/>
-      <c r="K86" s="47"/>
+      <c r="I86" s="35"/>
+      <c r="K86" s="35"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I87" s="47">
-        <f t="shared" ref="I87:K87" si="8">I71-I82</f>
+      <c r="I87" s="35">
+        <f t="shared" ref="I87:J87" si="10">I71-I82</f>
         <v>95.521000000000015</v>
       </c>
       <c r="J87" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>107.15099999999998</v>
       </c>
-      <c r="K87" s="47">
+      <c r="K87" s="35">
         <f>K71-K82</f>
         <v>159.214</v>
       </c>
@@ -4183,15 +4183,15 @@
       <c r="B88" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I88" s="47">
-        <f t="shared" ref="I88:J88" si="9">I87+I82</f>
+      <c r="I88" s="35">
+        <f t="shared" ref="I88:J88" si="11">I87+I82</f>
         <v>126.78400000000002</v>
       </c>
       <c r="J88" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>147.40199999999999</v>
       </c>
-      <c r="K88" s="47">
+      <c r="K88" s="35">
         <f>K87+K82</f>
         <v>265.35399999999998</v>
       </c>
@@ -4200,15 +4200,15 @@
       <c r="B90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I90" s="47">
-        <f t="shared" ref="I90:K90" si="10">+I69</f>
+      <c r="I90" s="35">
+        <f t="shared" ref="I90:J90" si="12">+I69</f>
         <v>34.429000000000002</v>
       </c>
-      <c r="J90" s="47">
-        <f t="shared" si="10"/>
+      <c r="J90" s="35">
+        <f t="shared" si="12"/>
         <v>32.843000000000004</v>
       </c>
-      <c r="K90" s="47">
+      <c r="K90" s="35">
         <f>+K69</f>
         <v>42.207000000000001</v>
       </c>
@@ -4217,15 +4217,15 @@
       <c r="B91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I91" s="47">
-        <f t="shared" ref="I91:K91" si="11">+I80</f>
+      <c r="I91" s="35">
+        <f t="shared" ref="I91:J91" si="13">+I80</f>
         <v>0</v>
       </c>
-      <c r="J91" s="47">
-        <f t="shared" si="11"/>
+      <c r="J91" s="35">
+        <f t="shared" si="13"/>
         <v>3.7</v>
       </c>
-      <c r="K91" s="47">
+      <c r="K91" s="35">
         <f>+K80</f>
         <v>6.4249999999999998</v>
       </c>
@@ -4234,16 +4234,16 @@
       <c r="B92" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E92" s="43"/>
-      <c r="I92" s="46">
-        <f t="shared" ref="I92:J92" si="12">I90-I91</f>
+      <c r="E92" s="31"/>
+      <c r="I92" s="34">
+        <f t="shared" ref="I92:J92" si="14">I90-I91</f>
         <v>34.429000000000002</v>
       </c>
-      <c r="J92" s="46">
-        <f t="shared" si="12"/>
+      <c r="J92" s="34">
+        <f t="shared" si="14"/>
         <v>29.143000000000004</v>
       </c>
-      <c r="K92" s="46">
+      <c r="K92" s="34">
         <f>K90-K91</f>
         <v>35.782000000000004</v>
       </c>

</xml_diff>

<commit_message>
£RPI price action update
</commit_message>
<xml_diff>
--- a/£RPI.xlsx
+++ b/£RPI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC5077E-6446-4BF9-BE5A-D9E3A2540C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB979D38-42C7-4344-9C62-3E46FAB3690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{455D1B8A-3F91-4588-9B7A-FCB01F8FFD95}"/>
   </bookViews>
@@ -21,6 +21,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -996,6 +1005,8 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1038,8 +1049,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2508,7 +2517,7 @@
   <dimension ref="A2:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2552,27 +2561,27 @@
       <c r="P3" s="23"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
-      <c r="G5" s="89" t="s">
+      <c r="C5" s="92"/>
+      <c r="D5" s="93"/>
+      <c r="G5" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="91"/>
-      <c r="Q5" s="92" t="s">
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="93"/>
+      <c r="Q5" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
       <c r="X5" s="24" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>6.44</v>
+        <v>7.22</v>
       </c>
       <c r="D6" s="13"/>
       <c r="G6" s="7"/>
@@ -2593,12 +2602,12 @@
       <c r="L6" s="61"/>
       <c r="M6" s="61"/>
       <c r="N6" s="59"/>
-      <c r="Q6" s="84" t="s">
+      <c r="Q6" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -2631,9 +2640,9 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="95">
+      <c r="C8" s="81">
         <f>C6*C7</f>
-        <v>1245.5972046000002</v>
+        <v>1396.4614623</v>
       </c>
       <c r="D8" s="13"/>
       <c r="G8" s="60">
@@ -2662,7 +2671,7 @@
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="95">
+      <c r="C9" s="81">
         <f>+'Financial Model'!F90*$C$13</f>
         <v>30.704000000000001</v>
       </c>
@@ -2686,7 +2695,7 @@
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="95">
+      <c r="C10" s="81">
         <f>+'Financial Model'!F91*$C$13</f>
         <v>4.4079999999999995</v>
       </c>
@@ -2720,7 +2729,7 @@
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="95">
+      <c r="C11" s="81">
         <f>C9-C10</f>
         <v>26.295999999999999</v>
       </c>
@@ -2747,9 +2756,9 @@
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="96">
+      <c r="C12" s="82">
         <f>C8-C11</f>
-        <v>1219.3012046000001</v>
+        <v>1370.1654622999999</v>
       </c>
       <c r="D12" s="14"/>
       <c r="G12" s="60">
@@ -2815,11 +2824,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="93"/>
       <c r="G15" s="7"/>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -2836,10 +2845,10 @@
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="81" t="s">
+      <c r="C16" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="82"/>
+      <c r="D16" s="84"/>
       <c r="G16" s="60">
         <v>45444</v>
       </c>
@@ -2852,21 +2861,21 @@
       <c r="L16" s="61"/>
       <c r="M16" s="61"/>
       <c r="N16" s="59"/>
-      <c r="Q16" s="84" t="s">
+      <c r="Q16" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
+      <c r="R16" s="86"/>
+      <c r="S16" s="86"/>
+      <c r="T16" s="86"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="82"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="1" t="s">
         <v>160</v>
       </c>
@@ -2889,8 +2898,8 @@
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="84"/>
       <c r="G18" s="7"/>
       <c r="H18" s="61"/>
       <c r="I18" s="61"/>
@@ -2910,8 +2919,8 @@
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="94"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
       <c r="G19" s="7"/>
       <c r="H19" s="61"/>
       <c r="I19" s="61"/>
@@ -2954,11 +2963,11 @@
       <c r="X21" s="41"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="90"/>
-      <c r="D22" s="91"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="93"/>
       <c r="G22" s="7">
         <v>2012</v>
       </c>
@@ -2971,21 +2980,21 @@
       <c r="L22" s="61"/>
       <c r="M22" s="61"/>
       <c r="N22" s="59"/>
-      <c r="Q22" s="84" t="s">
+      <c r="Q22" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
-      <c r="T22" s="84"/>
+      <c r="R22" s="86"/>
+      <c r="S22" s="86"/>
+      <c r="T22" s="86"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="82"/>
+      <c r="D23" s="84"/>
       <c r="G23" s="7"/>
       <c r="H23" s="61"/>
       <c r="I23" s="61"/>
@@ -3002,10 +3011,10 @@
       <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="81">
+      <c r="C24" s="83">
         <v>2012</v>
       </c>
-      <c r="D24" s="82"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="47" t="s">
         <v>130</v>
       </c>
@@ -3029,10 +3038,10 @@
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="83">
+      <c r="C25" s="85">
         <v>45444</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="84"/>
       <c r="G25" s="8"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
@@ -3047,30 +3056,30 @@
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="82"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="84"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="81">
+      <c r="C27" s="83">
         <f>+'Financial Model'!F50</f>
         <v>115</v>
       </c>
-      <c r="D27" s="82"/>
+      <c r="D27" s="84"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="G28" s="37"/>
-      <c r="Q28" s="84" t="s">
+      <c r="Q28" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="R28" s="84"/>
-      <c r="S28" s="84"/>
-      <c r="T28" s="84"/>
+      <c r="R28" s="86"/>
+      <c r="S28" s="86"/>
+      <c r="T28" s="86"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
@@ -3098,18 +3107,18 @@
       <c r="B31" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="88"/>
+      <c r="D31" s="90"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="Q32" s="84" t="s">
+      <c r="Q32" s="86" t="s">
         <v>155</v>
       </c>
-      <c r="R32" s="84"/>
-      <c r="S32" s="84"/>
-      <c r="T32" s="84"/>
+      <c r="R32" s="86"/>
+      <c r="S32" s="86"/>
+      <c r="T32" s="86"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q33" s="1" t="s">
@@ -3117,61 +3126,61 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="89" t="s">
+      <c r="B34" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="90"/>
-      <c r="D34" s="91"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="85">
+      <c r="C35" s="87">
         <f>C6/'Financial Model'!F88</f>
-        <v>6.1785575625</v>
-      </c>
-      <c r="D35" s="86"/>
+        <v>6.9268921741071425</v>
+      </c>
+      <c r="D35" s="88"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="85">
+      <c r="C36" s="87">
         <f>(C8*(1/C13))/SUM('Financial Model'!E13:F13)</f>
-        <v>5.11375672865318</v>
-      </c>
-      <c r="D36" s="86"/>
+        <v>5.7331247796391231</v>
+      </c>
+      <c r="D36" s="88"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="85">
+      <c r="C37" s="87">
         <f>(C12*(1/C13))/SUM('Financial Model'!E13:F13)</f>
-        <v>5.0057993998794315</v>
-      </c>
-      <c r="D37" s="86"/>
+        <v>5.6251674508653746</v>
+      </c>
+      <c r="D37" s="88"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="85">
+      <c r="C38" s="87">
         <f>+C6/('Financial Model'!K26*Main!C13)</f>
-        <v>29.853284389232297</v>
-      </c>
-      <c r="D38" s="86"/>
+        <v>33.469054858735582</v>
+      </c>
+      <c r="D38" s="88"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="85">
+      <c r="C39" s="87">
         <f>C12/('Financial Model'!K25*Main!C13)</f>
-        <v>50.815396245507337</v>
-      </c>
-      <c r="D39" s="86"/>
+        <v>57.102790209679448</v>
+      </c>
+      <c r="D39" s="88"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="80">
@@ -3180,10 +3189,10 @@
       <c r="B40" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="81">
+      <c r="C40" s="83">
         <v>42</v>
       </c>
-      <c r="D40" s="82"/>
+      <c r="D40" s="84"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B41" s="7"/>

</xml_diff>

<commit_message>
£RPI insider sale update
</commit_message>
<xml_diff>
--- a/£RPI.xlsx
+++ b/£RPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB979D38-42C7-4344-9C62-3E46FAB3690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88BB919-3F18-4C3A-A5ED-8A061CC4D54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{455D1B8A-3F91-4588-9B7A-FCB01F8FFD95}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="162">
   <si>
     <t>£RPI</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>Prev. Dovetail, Time Out</t>
+  </si>
+  <si>
+    <t>Elizabeth Upton (Dr's wife) sells 30,000 shares @ 619.57 (£185,872)</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1016,25 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1031,22 +1049,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2517,7 +2520,7 @@
   <dimension ref="A2:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G6" sqref="G6:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2561,27 +2564,27 @@
       <c r="P3" s="23"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="93"/>
-      <c r="G5" s="91" t="s">
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
+      <c r="G5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="93"/>
-      <c r="Q5" s="94" t="s">
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="91"/>
+      <c r="Q5" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
       <c r="X5" s="24" t="s">
         <v>29</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>7.22</v>
+        <v>5.71</v>
       </c>
       <c r="D6" s="13"/>
       <c r="G6" s="7"/>
@@ -2642,14 +2645,14 @@
       </c>
       <c r="C8" s="81">
         <f>C6*C7</f>
-        <v>1396.4614623</v>
+        <v>1104.4037326499999</v>
       </c>
       <c r="D8" s="13"/>
       <c r="G8" s="60">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="H8" s="61" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I8" s="61"/>
       <c r="J8" s="61"/>
@@ -2704,10 +2707,10 @@
         <v>H124</v>
       </c>
       <c r="G10" s="60">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="H10" s="61" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="I10" s="61"/>
       <c r="J10" s="61"/>
@@ -2758,14 +2761,14 @@
       </c>
       <c r="C12" s="82">
         <f>C8-C11</f>
-        <v>1370.1654622999999</v>
+        <v>1078.1077326499999</v>
       </c>
       <c r="D12" s="14"/>
       <c r="G12" s="60">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="H12" s="61" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
@@ -2808,10 +2811,10 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G14" s="60">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="H14" s="61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" s="61"/>
       <c r="J14" s="61"/>
@@ -2824,11 +2827,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="92"/>
-      <c r="D15" s="93"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="91"/>
       <c r="G15" s="7"/>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -2850,10 +2853,10 @@
       </c>
       <c r="D16" s="84"/>
       <c r="G16" s="60">
-        <v>45444</v>
+        <v>45505</v>
       </c>
       <c r="H16" s="61" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="I16" s="61"/>
       <c r="J16" s="61"/>
@@ -2900,8 +2903,12 @@
       </c>
       <c r="C18" s="83"/>
       <c r="D18" s="84"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="61"/>
+      <c r="G18" s="60">
+        <v>45444</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>36</v>
+      </c>
       <c r="I18" s="61"/>
       <c r="J18" s="61"/>
       <c r="K18" s="61"/>
@@ -2919,8 +2926,8 @@
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="96"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="88"/>
       <c r="G19" s="7"/>
       <c r="H19" s="61"/>
       <c r="I19" s="61"/>
@@ -2963,11 +2970,11 @@
       <c r="X21" s="41"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="92"/>
-      <c r="D22" s="93"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
       <c r="G22" s="7">
         <v>2012</v>
       </c>
@@ -3038,7 +3045,7 @@
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="85">
+      <c r="C25" s="96">
         <v>45444</v>
       </c>
       <c r="D25" s="84"/>
@@ -3107,10 +3114,10 @@
       <c r="B31" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="89" t="s">
+      <c r="C31" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="90"/>
+      <c r="D31" s="95"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="Q32" s="86" t="s">
@@ -3126,61 +3133,61 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="93"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="91"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="87">
+      <c r="C35" s="92">
         <f>C6/'Financial Model'!F88</f>
-        <v>6.9268921741071425</v>
-      </c>
-      <c r="D35" s="88"/>
+        <v>5.4781931183035715</v>
+      </c>
+      <c r="D35" s="93"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="87">
+      <c r="C36" s="92">
         <f>(C8*(1/C13))/SUM('Financial Model'!E13:F13)</f>
-        <v>5.7331247796391231</v>
-      </c>
-      <c r="D36" s="88"/>
+        <v>4.5340917578586417</v>
+      </c>
+      <c r="D36" s="93"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="87">
+      <c r="C37" s="92">
         <f>(C12*(1/C13))/SUM('Financial Model'!E13:F13)</f>
-        <v>5.6251674508653746</v>
-      </c>
-      <c r="D37" s="88"/>
+        <v>4.4261344290848923</v>
+      </c>
+      <c r="D37" s="93"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="87">
+      <c r="C38" s="92">
         <f>+C6/('Financial Model'!K26*Main!C13)</f>
-        <v>33.469054858735582</v>
-      </c>
-      <c r="D38" s="88"/>
+        <v>26.469294078030497</v>
+      </c>
+      <c r="D38" s="93"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="87">
+      <c r="C39" s="92">
         <f>C12/('Financial Model'!K25*Main!C13)</f>
-        <v>57.102790209679448</v>
-      </c>
-      <c r="D39" s="88"/>
+        <v>44.931040355961635</v>
+      </c>
+      <c r="D39" s="93"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="80">
@@ -3206,6 +3213,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="Q32:T32"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="Q28:T28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="Q5:T5"/>
     <mergeCell ref="Q6:T6"/>
@@ -3222,17 +3240,6 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="Q28:T28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="Q32:T32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{C8D4D434-582F-463A-A9FE-87E24B6B9D24}"/>
@@ -3251,7 +3258,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>